<commit_message>
work order look ok
</commit_message>
<xml_diff>
--- a/mediafiles/cmms-pon.xlsx
+++ b/mediafiles/cmms-pon.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\djangoProjects\cmms_pon\mediafiles\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD80143-1BFA-4301-B9B1-928923B02FB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="DbSetup" sheetId="42" r:id="rId1"/>
@@ -22,6 +16,7 @@
     <sheet name="mode" sheetId="38" r:id="rId7"/>
     <sheet name="action" sheetId="37" r:id="rId8"/>
     <sheet name="Category" sheetId="41" r:id="rId9"/>
+    <sheet name="Wo priority" sheetId="43" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="sort" localSheetId="8">#REF!</definedName>
@@ -58,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="105">
   <si>
     <t>Safety</t>
   </si>
@@ -361,12 +356,24 @@
   </si>
   <si>
     <t>Mode</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Shutdown</t>
+  </si>
+  <si>
+    <t>Emergency</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="10"/>
@@ -455,7 +462,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -482,7 +489,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -541,7 +548,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -574,26 +581,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -626,23 +616,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -818,7 +791,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -880,8 +853,66 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -981,7 +1012,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -1157,14 +1188,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1173,7 +1204,7 @@
     <col min="2" max="2" width="85.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1324,14 +1355,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1385,7 +1416,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -1575,7 +1606,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -1616,14 +1647,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1920,7 +1951,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>

</xml_diff>